<commit_message>
fixed data format of result
</commit_message>
<xml_diff>
--- a/wyniki_kendall.xlsx
+++ b/wyniki_kendall.xlsx
@@ -1255,7 +1255,7 @@
         <v>2</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M2">
         <v>260</v>
@@ -1323,7 +1323,7 @@
         <v>2</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M3">
         <v>235</v>
@@ -1391,7 +1391,7 @@
         <v>2</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M4">
         <v>240</v>
@@ -1459,7 +1459,7 @@
         <v>2</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>5.3</v>
       </c>
       <c r="M5">
         <v>200</v>
@@ -1527,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>6.4</v>
       </c>
       <c r="M6">
         <v>250</v>
@@ -1595,7 +1595,7 @@
         <v>2</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>6.6</v>
       </c>
       <c r="M7">
         <v>250</v>
@@ -1663,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="L8">
-        <v>2</v>
+        <v>6.2</v>
       </c>
       <c r="M8">
         <v>250</v>
@@ -1731,7 +1731,7 @@
         <v>2</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>4.3</v>
       </c>
       <c r="M9">
         <v>250</v>
@@ -1799,7 +1799,7 @@
         <v>2</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="M10">
         <v>250</v>
@@ -1867,7 +1867,7 @@
         <v>2</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>6.3</v>
       </c>
       <c r="M11">
         <v>250</v>
@@ -1935,7 +1935,7 @@
         <v>2</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="M12">
         <v>230</v>
@@ -2003,7 +2003,7 @@
         <v>2</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>5.9</v>
       </c>
       <c r="M13">
         <v>250</v>
@@ -2071,7 +2071,7 @@
         <v>2</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>8.4</v>
       </c>
       <c r="M14">
         <v>243</v>
@@ -2139,7 +2139,7 @@
         <v>2</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="M15">
         <v>222</v>
@@ -2207,7 +2207,7 @@
         <v>2</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="M16">
         <v>280</v>
@@ -2275,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="M17">
         <v>193</v>
@@ -2343,7 +2343,7 @@
         <v>2</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>7.4</v>
       </c>
       <c r="M18">
         <v>234</v>
@@ -2411,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="L19">
-        <v>2</v>
+        <v>4.4</v>
       </c>
       <c r="M19">
         <v>250</v>
@@ -2479,7 +2479,7 @@
         <v>2</v>
       </c>
       <c r="L20">
-        <v>2</v>
+        <v>7.3</v>
       </c>
       <c r="M20">
         <v>225</v>
@@ -2547,7 +2547,7 @@
         <v>2</v>
       </c>
       <c r="L21">
-        <v>2</v>
+        <v>7.5</v>
       </c>
       <c r="M21">
         <v>218</v>
@@ -2615,7 +2615,7 @@
         <v>2</v>
       </c>
       <c r="L22">
-        <v>2</v>
+        <v>6.1</v>
       </c>
       <c r="M22">
         <v>250</v>
@@ -2683,7 +2683,7 @@
         <v>2</v>
       </c>
       <c r="L23">
-        <v>2</v>
+        <v>4.8</v>
       </c>
       <c r="M23">
         <v>306</v>
@@ -2751,7 +2751,7 @@
         <v>2</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>7.6</v>
       </c>
       <c r="M24">
         <v>240</v>
@@ -2819,7 +2819,7 @@
         <v>2</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M25">
         <v>250</v>
@@ -2887,7 +2887,7 @@
         <v>2</v>
       </c>
       <c r="L26">
-        <v>2</v>
+        <v>7.2</v>
       </c>
       <c r="M26">
         <v>213</v>
@@ -2955,7 +2955,7 @@
         <v>3</v>
       </c>
       <c r="L27">
-        <v>3</v>
+        <v>7.1</v>
       </c>
       <c r="M27">
         <v>240</v>
@@ -3023,7 +3023,7 @@
         <v>2</v>
       </c>
       <c r="L28">
-        <v>2</v>
+        <v>5.8</v>
       </c>
       <c r="M28">
         <v>250</v>
@@ -3091,7 +3091,7 @@
         <v>2</v>
       </c>
       <c r="L29">
-        <v>2</v>
+        <v>5.9</v>
       </c>
       <c r="M29">
         <v>244</v>
@@ -3159,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>5.3</v>
       </c>
       <c r="M30">
         <v>250</v>
@@ -3227,7 +3227,7 @@
         <v>2</v>
       </c>
       <c r="L31">
-        <v>2</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="M31">
         <v>190</v>
@@ -3295,7 +3295,7 @@
         <v>2</v>
       </c>
       <c r="L32">
-        <v>2</v>
+        <v>6.1</v>
       </c>
       <c r="M32">
         <v>250</v>
@@ -3363,7 +3363,7 @@
         <v>2</v>
       </c>
       <c r="L33">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M33">
         <v>182</v>
@@ -3431,7 +3431,7 @@
         <v>2</v>
       </c>
       <c r="L34">
-        <v>2</v>
+        <v>4.8</v>
       </c>
       <c r="M34">
         <v>260</v>
@@ -3499,7 +3499,7 @@
         <v>2</v>
       </c>
       <c r="L35">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="M35">
         <v>250</v>
@@ -3567,7 +3567,7 @@
         <v>2</v>
       </c>
       <c r="L36">
-        <v>2</v>
+        <v>8.1</v>
       </c>
       <c r="M36">
         <v>202</v>
@@ -3635,7 +3635,7 @@
         <v>2</v>
       </c>
       <c r="L37">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="M37">
         <v>270</v>
@@ -3703,7 +3703,7 @@
         <v>5</v>
       </c>
       <c r="L38">
-        <v>5</v>
+        <v>6.1</v>
       </c>
       <c r="M38">
         <v>250</v>
@@ -3771,7 +3771,7 @@
         <v>2</v>
       </c>
       <c r="L39">
-        <v>2</v>
+        <v>6.3</v>
       </c>
       <c r="M39">
         <v>240</v>
@@ -3839,7 +3839,7 @@
         <v>2</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M40">
         <v>190</v>
@@ -3907,7 +3907,7 @@
         <v>2</v>
       </c>
       <c r="L41">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="M41">
         <v>268</v>
@@ -3975,7 +3975,7 @@
         <v>2</v>
       </c>
       <c r="L42">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="M42">
         <v>250</v>
@@ -4043,7 +4043,7 @@
         <v>2</v>
       </c>
       <c r="L43">
-        <v>2</v>
+        <v>7.8</v>
       </c>
       <c r="M43">
         <v>236</v>
@@ -4111,7 +4111,7 @@
         <v>3</v>
       </c>
       <c r="L44">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="M44">
         <v>250</v>
@@ -4179,7 +4179,7 @@
         <v>2</v>
       </c>
       <c r="L45">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="M45">
         <v>304</v>
@@ -4247,7 +4247,7 @@
         <v>4</v>
       </c>
       <c r="L46">
-        <v>4</v>
+        <v>6.1</v>
       </c>
       <c r="M46">
         <v>250</v>
@@ -4315,7 +4315,7 @@
         <v>4</v>
       </c>
       <c r="L47">
-        <v>4</v>
+        <v>5.2</v>
       </c>
       <c r="M47">
         <v>255</v>
@@ -4383,7 +4383,7 @@
         <v>2</v>
       </c>
       <c r="L48">
-        <v>2</v>
+        <v>6.5</v>
       </c>
       <c r="M48">
         <v>201</v>
@@ -4451,7 +4451,7 @@
         <v>4</v>
       </c>
       <c r="L49">
-        <v>4</v>
+        <v>5.9</v>
       </c>
       <c r="M49">
         <v>250</v>
@@ -4519,7 +4519,7 @@
         <v>2</v>
       </c>
       <c r="L50">
-        <v>2</v>
+        <v>6.4</v>
       </c>
       <c r="M50">
         <v>193</v>
@@ -4587,7 +4587,7 @@
         <v>2</v>
       </c>
       <c r="L51">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M51">
         <v>290</v>
@@ -4655,7 +4655,7 @@
         <v>4</v>
       </c>
       <c r="L52">
-        <v>4</v>
+        <v>6.2</v>
       </c>
       <c r="M52">
         <v>233</v>
@@ -4723,7 +4723,7 @@
         <v>4</v>
       </c>
       <c r="L53">
-        <v>4</v>
+        <v>5.2</v>
       </c>
       <c r="M53">
         <v>250</v>
@@ -4791,7 +4791,7 @@
         <v>2</v>
       </c>
       <c r="L54">
-        <v>2</v>
+        <v>5.3</v>
       </c>
       <c r="M54">
         <v>285</v>
@@ -4859,7 +4859,7 @@
         <v>2</v>
       </c>
       <c r="L55">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="M55">
         <v>250</v>
@@ -4927,7 +4927,7 @@
         <v>2</v>
       </c>
       <c r="L56">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M56">
         <v>226</v>
@@ -4995,7 +4995,7 @@
         <v>2</v>
       </c>
       <c r="L57">
-        <v>2</v>
+        <v>6.9</v>
       </c>
       <c r="M57">
         <v>225</v>
@@ -5063,7 +5063,7 @@
         <v>2</v>
       </c>
       <c r="L58">
-        <v>2</v>
+        <v>6.6</v>
       </c>
       <c r="M58">
         <v>250</v>
@@ -5131,7 +5131,7 @@
         <v>5</v>
       </c>
       <c r="L59">
-        <v>5</v>
+        <v>5.8</v>
       </c>
       <c r="M59">
         <v>272</v>
@@ -5199,7 +5199,7 @@
         <v>5</v>
       </c>
       <c r="L60">
-        <v>5</v>
+        <v>6.4</v>
       </c>
       <c r="M60">
         <v>247</v>
@@ -5267,7 +5267,7 @@
         <v>2</v>
       </c>
       <c r="L61">
-        <v>2</v>
+        <v>4.6</v>
       </c>
       <c r="M61">
         <v>290</v>
@@ -5335,7 +5335,7 @@
         <v>4</v>
       </c>
       <c r="L62">
-        <v>4</v>
+        <v>5.4</v>
       </c>
       <c r="M62">
         <v>255</v>
@@ -5403,7 +5403,7 @@
         <v>4</v>
       </c>
       <c r="L63">
-        <v>4</v>
+        <v>7.8</v>
       </c>
       <c r="M63">
         <v>212</v>
@@ -5471,7 +5471,7 @@
         <v>2</v>
       </c>
       <c r="L64">
-        <v>2</v>
+        <v>5.4</v>
       </c>
       <c r="M64">
         <v>215</v>
@@ -5539,7 +5539,7 @@
         <v>5</v>
       </c>
       <c r="L65">
-        <v>5</v>
+        <v>6.4</v>
       </c>
       <c r="M65">
         <v>250</v>
@@ -5607,7 +5607,7 @@
         <v>4</v>
       </c>
       <c r="L66">
-        <v>4</v>
+        <v>4.9</v>
       </c>
       <c r="M66">
         <v>270</v>
@@ -5675,7 +5675,7 @@
         <v>5</v>
       </c>
       <c r="L67">
-        <v>5</v>
+        <v>5.6</v>
       </c>
       <c r="M67">
         <v>275</v>
@@ -5743,7 +5743,7 @@
         <v>3</v>
       </c>
       <c r="L68">
-        <v>3</v>
+        <v>6.9</v>
       </c>
       <c r="M68">
         <v>240</v>
@@ -5811,7 +5811,7 @@
         <v>5</v>
       </c>
       <c r="L69">
-        <v>5</v>
+        <v>6.8</v>
       </c>
       <c r="M69">
         <v>242</v>
@@ -5879,7 +5879,7 @@
         <v>3</v>
       </c>
       <c r="L70">
-        <v>3</v>
+        <v>6.8</v>
       </c>
       <c r="M70">
         <v>241</v>
@@ -5947,7 +5947,7 @@
         <v>2</v>
       </c>
       <c r="L71">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M71">
         <v>186</v>
@@ -6015,7 +6015,7 @@
         <v>2</v>
       </c>
       <c r="L72">
-        <v>2</v>
+        <v>3.7</v>
       </c>
       <c r="M72">
         <v>290</v>
@@ -6083,7 +6083,7 @@
         <v>4</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>5.2</v>
       </c>
       <c r="M73">
         <v>250</v>
@@ -6151,7 +6151,7 @@
         <v>2</v>
       </c>
       <c r="L74">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="M74">
         <v>302</v>
@@ -6219,7 +6219,7 @@
         <v>4</v>
       </c>
       <c r="L75">
-        <v>4</v>
+        <v>7.6</v>
       </c>
       <c r="M75">
         <v>232</v>
@@ -6287,7 +6287,7 @@
         <v>4</v>
       </c>
       <c r="L76">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="M76">
         <v>250</v>
@@ -6355,7 +6355,7 @@
         <v>2</v>
       </c>
       <c r="L77">
-        <v>2</v>
+        <v>4.9</v>
       </c>
       <c r="M77">
         <v>249</v>
@@ -6423,7 +6423,7 @@
         <v>3</v>
       </c>
       <c r="L78">
-        <v>3</v>
+        <v>7.2</v>
       </c>
       <c r="M78">
         <v>243</v>
@@ -6491,7 +6491,7 @@
         <v>5</v>
       </c>
       <c r="L79">
-        <v>5</v>
+        <v>6.9</v>
       </c>
       <c r="M79">
         <v>240</v>
@@ -6559,7 +6559,7 @@
         <v>5</v>
       </c>
       <c r="L80">
-        <v>5</v>
+        <v>6.7</v>
       </c>
       <c r="M80">
         <v>230</v>
@@ -6627,7 +6627,7 @@
         <v>2</v>
       </c>
       <c r="L81">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M81">
         <v>304</v>
@@ -6695,7 +6695,7 @@
         <v>2</v>
       </c>
       <c r="L82">
-        <v>2</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="M82">
         <v>237</v>
@@ -6763,7 +6763,7 @@
         <v>2</v>
       </c>
       <c r="L83">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="M83">
         <v>275</v>
@@ -6831,7 +6831,7 @@
         <v>2</v>
       </c>
       <c r="L84">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M84">
         <v>314</v>
@@ -6899,7 +6899,7 @@
         <v>2</v>
       </c>
       <c r="L85">
-        <v>2</v>
+        <v>5.4</v>
       </c>
       <c r="M85">
         <v>275</v>
@@ -6967,7 +6967,7 @@
         <v>2</v>
       </c>
       <c r="L86">
-        <v>2</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="M86">
         <v>200</v>
@@ -7035,7 +7035,7 @@
         <v>2</v>
       </c>
       <c r="L87">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="M87">
         <v>250</v>
@@ -7103,7 +7103,7 @@
         <v>3</v>
       </c>
       <c r="L88">
-        <v>3</v>
+        <v>4.8</v>
       </c>
       <c r="M88">
         <v>248</v>
@@ -7171,7 +7171,7 @@
         <v>4</v>
       </c>
       <c r="L89">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="M89">
         <v>250</v>
@@ -7239,7 +7239,7 @@
         <v>4</v>
       </c>
       <c r="L90">
-        <v>4</v>
+        <v>6.2</v>
       </c>
       <c r="M90">
         <v>230</v>
@@ -7307,7 +7307,7 @@
         <v>2</v>
       </c>
       <c r="L91">
-        <v>2</v>
+        <v>7.8</v>
       </c>
       <c r="M91">
         <v>201</v>
@@ -7375,7 +7375,7 @@
         <v>4</v>
       </c>
       <c r="L92">
-        <v>4</v>
+        <v>5.6</v>
       </c>
       <c r="M92">
         <v>274</v>
@@ -7443,7 +7443,7 @@
         <v>4</v>
       </c>
       <c r="L93">
-        <v>4</v>
+        <v>5.9</v>
       </c>
       <c r="M93">
         <v>250</v>
@@ -7511,7 +7511,7 @@
         <v>2</v>
       </c>
       <c r="L94">
-        <v>2</v>
+        <v>5.4</v>
       </c>
       <c r="M94">
         <v>275</v>
@@ -7579,7 +7579,7 @@
         <v>3</v>
       </c>
       <c r="L95">
-        <v>3</v>
+        <v>6.9</v>
       </c>
       <c r="M95">
         <v>227</v>
@@ -7647,7 +7647,7 @@
         <v>2</v>
       </c>
       <c r="L96">
-        <v>2</v>
+        <v>5.1</v>
       </c>
       <c r="M96">
         <v>280</v>
@@ -7715,7 +7715,7 @@
         <v>4</v>
       </c>
       <c r="L97">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M97">
         <v>240</v>
@@ -7783,7 +7783,7 @@
         <v>4</v>
       </c>
       <c r="L98">
-        <v>4</v>
+        <v>6.9</v>
       </c>
       <c r="M98">
         <v>245</v>
@@ -7851,7 +7851,7 @@
         <v>2</v>
       </c>
       <c r="L99">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M99">
         <v>185</v>
@@ -7919,7 +7919,7 @@
         <v>2</v>
       </c>
       <c r="L100">
-        <v>2</v>
+        <v>4.9</v>
       </c>
       <c r="M100">
         <v>243</v>
@@ -7987,7 +7987,7 @@
         <v>2</v>
       </c>
       <c r="L101">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="M101">
         <v>296</v>
@@ -8055,7 +8055,7 @@
         <v>2</v>
       </c>
       <c r="L102">
-        <v>2</v>
+        <v>6.2</v>
       </c>
       <c r="M102">
         <v>265</v>
@@ -8123,7 +8123,7 @@
         <v>2</v>
       </c>
       <c r="L103">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="M103">
         <v>275</v>
@@ -8191,7 +8191,7 @@
         <v>2</v>
       </c>
       <c r="L104">
-        <v>2</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="M104">
         <v>209</v>
@@ -8259,7 +8259,7 @@
         <v>2</v>
       </c>
       <c r="L105">
-        <v>2</v>
+        <v>4.7</v>
       </c>
       <c r="M105">
         <v>280</v>
@@ -8327,7 +8327,7 @@
         <v>2</v>
       </c>
       <c r="L106">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M106">
         <v>304</v>
@@ -8395,7 +8395,7 @@
         <v>2</v>
       </c>
       <c r="L107">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="M107">
         <v>346</v>
@@ -8463,7 +8463,7 @@
         <v>2</v>
       </c>
       <c r="L108">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="M108">
         <v>322</v>
@@ -8531,7 +8531,7 @@
         <v>3</v>
       </c>
       <c r="L109">
-        <v>3</v>
+        <v>6.7</v>
       </c>
       <c r="M109">
         <v>204</v>
@@ -8599,7 +8599,7 @@
         <v>3</v>
       </c>
       <c r="L110">
-        <v>3</v>
+        <v>5.3</v>
       </c>
       <c r="M110">
         <v>275</v>
@@ -8667,7 +8667,7 @@
         <v>2</v>
       </c>
       <c r="L111">
-        <v>2</v>
+        <v>7.4</v>
       </c>
       <c r="M111">
         <v>225</v>
@@ -8735,7 +8735,7 @@
         <v>4</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>7.9</v>
       </c>
       <c r="M112">
         <v>200</v>
@@ -8803,7 +8803,7 @@
         <v>2</v>
       </c>
       <c r="L113">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="M113">
         <v>243</v>
@@ -8871,7 +8871,7 @@
         <v>2</v>
       </c>
       <c r="L114">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="M114">
         <v>225</v>
@@ -8939,7 +8939,7 @@
         <v>3</v>
       </c>
       <c r="L115">
-        <v>3</v>
+        <v>6.9</v>
       </c>
       <c r="M115">
         <v>229</v>
@@ -9075,7 +9075,7 @@
         <v>2</v>
       </c>
       <c r="L117">
-        <v>2</v>
+        <v>5.4</v>
       </c>
       <c r="M117">
         <v>272</v>
@@ -9143,7 +9143,7 @@
         <v>2</v>
       </c>
       <c r="L118">
-        <v>2</v>
+        <v>4.1</v>
       </c>
       <c r="M118">
         <v>260</v>
@@ -9211,7 +9211,7 @@
         <v>2</v>
       </c>
       <c r="L119">
-        <v>2</v>
+        <v>4.6</v>
       </c>
       <c r="M119">
         <v>250</v>
@@ -9279,7 +9279,7 @@
         <v>2</v>
       </c>
       <c r="L120">
-        <v>2</v>
+        <v>5.1</v>
       </c>
       <c r="M120">
         <v>298</v>
@@ -9347,7 +9347,7 @@
         <v>2</v>
       </c>
       <c r="L121">
-        <v>2</v>
+        <v>7.1</v>
       </c>
       <c r="M121">
         <v>238</v>
@@ -9415,7 +9415,7 @@
         <v>2</v>
       </c>
       <c r="L122">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="M122">
         <v>262</v>
@@ -9483,7 +9483,7 @@
         <v>2</v>
       </c>
       <c r="L123">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="M123">
         <v>289</v>
@@ -9551,7 +9551,7 @@
         <v>2</v>
       </c>
       <c r="L124">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="M124">
         <v>303</v>
@@ -9619,7 +9619,7 @@
         <v>2</v>
       </c>
       <c r="L125">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="M125">
         <v>331</v>
@@ -9687,7 +9687,7 @@
         <v>5</v>
       </c>
       <c r="L126">
-        <v>5</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="M126">
         <v>217</v>
@@ -9755,7 +9755,7 @@
         <v>3</v>
       </c>
       <c r="L127">
-        <v>3</v>
+        <v>7.4</v>
       </c>
       <c r="M127">
         <v>217</v>
@@ -9823,7 +9823,7 @@
         <v>2</v>
       </c>
       <c r="L128">
-        <v>2</v>
+        <v>4.8</v>
       </c>
       <c r="M128">
         <v>280</v>
@@ -9891,7 +9891,7 @@
         <v>2</v>
       </c>
       <c r="L129">
-        <v>2</v>
+        <v>5.4</v>
       </c>
       <c r="M129">
         <v>255</v>
@@ -9959,7 +9959,7 @@
         <v>2</v>
       </c>
       <c r="L130">
-        <v>2</v>
+        <v>7.6</v>
       </c>
       <c r="M130">
         <v>226</v>
@@ -10027,7 +10027,7 @@
         <v>2</v>
       </c>
       <c r="L131">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="M131">
         <v>290</v>
@@ -10095,7 +10095,7 @@
         <v>2</v>
       </c>
       <c r="L132">
-        <v>2</v>
+        <v>4.6</v>
       </c>
       <c r="M132">
         <v>250</v>
@@ -10163,7 +10163,7 @@
         <v>2</v>
       </c>
       <c r="L133">
-        <v>2</v>
+        <v>6.8</v>
       </c>
       <c r="M133">
         <v>221</v>
@@ -10231,7 +10231,7 @@
         <v>2</v>
       </c>
       <c r="L134">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M134">
         <v>260</v>
@@ -10299,7 +10299,7 @@
         <v>2</v>
       </c>
       <c r="L135">
-        <v>2</v>
+        <v>6.1</v>
       </c>
       <c r="M135">
         <v>176</v>
@@ -10367,7 +10367,7 @@
         <v>2</v>
       </c>
       <c r="L136">
-        <v>2</v>
+        <v>4.7</v>
       </c>
       <c r="M136">
         <v>250</v>
@@ -10435,7 +10435,7 @@
         <v>2</v>
       </c>
       <c r="L137">
-        <v>2</v>
+        <v>4.4</v>
       </c>
       <c r="M137">
         <v>255</v>
@@ -10503,7 +10503,7 @@
         <v>5</v>
       </c>
       <c r="L138">
-        <v>5</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="M138">
         <v>224</v>
@@ -10571,7 +10571,7 @@
         <v>3</v>
       </c>
       <c r="L139">
-        <v>3</v>
+        <v>5.1</v>
       </c>
       <c r="M139">
         <v>250</v>
@@ -10639,7 +10639,7 @@
         <v>2</v>
       </c>
       <c r="L140">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="M140">
         <v>315</v>
@@ -10707,7 +10707,7 @@
         <v>4</v>
       </c>
       <c r="L141">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M141">
         <v>216</v>
@@ -10775,7 +10775,7 @@
         <v>2</v>
       </c>
       <c r="L142">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="M142">
         <v>310</v>
@@ -10843,7 +10843,7 @@
         <v>2</v>
       </c>
       <c r="L143">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M143">
         <v>282</v>
@@ -10911,7 +10911,7 @@
         <v>5</v>
       </c>
       <c r="L144">
-        <v>5</v>
+        <v>3.9</v>
       </c>
       <c r="M144">
         <v>305</v>
@@ -10979,7 +10979,7 @@
         <v>2</v>
       </c>
       <c r="L145">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M145">
         <v>315</v>
@@ -11047,7 +11047,7 @@
         <v>2</v>
       </c>
       <c r="L146">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M146">
         <v>362</v>
@@ -11115,7 +11115,7 @@
         <v>2</v>
       </c>
       <c r="L147">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M147">
         <v>306</v>
@@ -11183,7 +11183,7 @@
         <v>2</v>
       </c>
       <c r="L148">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M148">
         <v>312</v>
@@ -11251,7 +11251,7 @@
         <v>2</v>
       </c>
       <c r="L149">
-        <v>2</v>
+        <v>3.7</v>
       </c>
       <c r="M149">
         <v>333</v>
@@ -11319,7 +11319,7 @@
         <v>2</v>
       </c>
       <c r="L150">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M150">
         <v>315</v>
@@ -11387,7 +11387,7 @@
         <v>3</v>
       </c>
       <c r="L151">
-        <v>3</v>
+        <v>6.3</v>
       </c>
       <c r="M151">
         <v>214</v>
@@ -11455,7 +11455,7 @@
         <v>3</v>
       </c>
       <c r="L152">
-        <v>3</v>
+        <v>6.4</v>
       </c>
       <c r="M152">
         <v>235</v>
@@ -11523,7 +11523,7 @@
         <v>2</v>
       </c>
       <c r="L153">
-        <v>2</v>
+        <v>5.3</v>
       </c>
       <c r="M153">
         <v>275</v>
@@ -11591,7 +11591,7 @@
         <v>2</v>
       </c>
       <c r="L154">
-        <v>2</v>
+        <v>4.3</v>
       </c>
       <c r="M154">
         <v>290</v>
@@ -11659,7 +11659,7 @@
         <v>2</v>
       </c>
       <c r="L155">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="M155">
         <v>341</v>
@@ -11727,7 +11727,7 @@
         <v>2</v>
       </c>
       <c r="L156">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M156">
         <v>310</v>
@@ -11795,7 +11795,7 @@
         <v>2</v>
       </c>
       <c r="L157">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="M157">
         <v>305</v>
@@ -11863,7 +11863,7 @@
         <v>2</v>
       </c>
       <c r="L158">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M158">
         <v>310</v>
@@ -11931,7 +11931,7 @@
         <v>2</v>
       </c>
       <c r="L159">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="M159">
         <v>306</v>
@@ -11999,7 +11999,7 @@
         <v>2</v>
       </c>
       <c r="L160">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="M160">
         <v>325</v>
@@ -12067,7 +12067,7 @@
         <v>4</v>
       </c>
       <c r="L161">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="M161">
         <v>306</v>
@@ -12135,7 +12135,7 @@
         <v>4</v>
       </c>
       <c r="L162">
-        <v>4</v>
+        <v>3.7</v>
       </c>
       <c r="M162">
         <v>322</v>
@@ -12203,7 +12203,7 @@
         <v>2</v>
       </c>
       <c r="L163">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="M163">
         <v>326</v>
@@ -12271,7 +12271,7 @@
         <v>2</v>
       </c>
       <c r="L164">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M164">
         <v>315</v>
@@ -12339,7 +12339,7 @@
         <v>2</v>
       </c>
       <c r="L165">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M165">
         <v>347</v>
@@ -12407,7 +12407,7 @@
         <v>2</v>
       </c>
       <c r="L166">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M166">
         <v>317</v>
@@ -12475,7 +12475,7 @@
         <v>2</v>
       </c>
       <c r="L167">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M167">
         <v>177</v>
@@ -12543,7 +12543,7 @@
         <v>2</v>
       </c>
       <c r="L168">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="M168">
         <v>258</v>
@@ -12611,7 +12611,7 @@
         <v>2</v>
       </c>
       <c r="L169">
-        <v>2</v>
+        <v>4.6</v>
       </c>
       <c r="M169">
         <v>302</v>
@@ -12679,7 +12679,7 @@
         <v>2</v>
       </c>
       <c r="L170">
-        <v>2</v>
+        <v>4.8</v>
       </c>
       <c r="M170">
         <v>314</v>
@@ -12747,7 +12747,7 @@
         <v>2</v>
       </c>
       <c r="L171">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M171">
         <v>325</v>
@@ -12815,7 +12815,7 @@
         <v>2</v>
       </c>
       <c r="L172">
-        <v>2</v>
+        <v>5.1</v>
       </c>
       <c r="M172">
         <v>212</v>
@@ -12883,7 +12883,7 @@
         <v>2</v>
       </c>
       <c r="L173">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M173">
         <v>306</v>
@@ -12951,7 +12951,7 @@
         <v>2</v>
       </c>
       <c r="L174">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="M174">
         <v>170</v>
@@ -13019,7 +13019,7 @@
         <v>2</v>
       </c>
       <c r="L175">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="M175">
         <v>340</v>
@@ -13087,7 +13087,7 @@
         <v>5</v>
       </c>
       <c r="L176">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="M176">
         <v>305</v>
@@ -13155,7 +13155,7 @@
         <v>4</v>
       </c>
       <c r="L177">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="M177">
         <v>215</v>
@@ -13223,7 +13223,7 @@
         <v>2</v>
       </c>
       <c r="L178">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M178">
         <v>274</v>
@@ -13291,7 +13291,7 @@
         <v>2</v>
       </c>
       <c r="L179">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="M179">
         <v>210</v>
@@ -13359,7 +13359,7 @@
         <v>2</v>
       </c>
       <c r="L180">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M180">
         <v>383</v>
@@ -13427,7 +13427,7 @@
         <v>2</v>
       </c>
       <c r="L181">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M181">
         <v>333</v>
@@ -13495,7 +13495,7 @@
         <v>2</v>
       </c>
       <c r="L182">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M182">
         <v>325</v>
@@ -13563,7 +13563,7 @@
         <v>2</v>
       </c>
       <c r="L183">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="M183">
         <v>360</v>
@@ -13631,7 +13631,7 @@
         <v>2</v>
       </c>
       <c r="L184">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M184">
         <v>318</v>
@@ -13699,7 +13699,7 @@
         <v>2</v>
       </c>
       <c r="L185">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M185">
         <v>332</v>
@@ -13767,7 +13767,7 @@
         <v>2</v>
       </c>
       <c r="L186">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="M186">
         <v>325</v>
@@ -13835,7 +13835,7 @@
         <v>2</v>
       </c>
       <c r="L187">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="M187">
         <v>330</v>
@@ -13903,7 +13903,7 @@
         <v>2</v>
       </c>
       <c r="L188">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="M188">
         <v>328</v>
@@ -13971,7 +13971,7 @@
         <v>5</v>
       </c>
       <c r="L189">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M189">
         <v>180</v>
@@ -14039,7 +14039,7 @@
         <v>3</v>
       </c>
       <c r="L190">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="M190">
         <v>298</v>
@@ -14107,7 +14107,7 @@
         <v>4</v>
       </c>
       <c r="L191">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="M191">
         <v>240</v>
@@ -14175,7 +14175,7 @@
         <v>3</v>
       </c>
       <c r="L192">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="M192">
         <v>154</v>
@@ -14243,7 +14243,7 @@
         <v>2</v>
       </c>
       <c r="L193">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M193">
         <v>350</v>
@@ -14311,7 +14311,7 @@
         <v>2</v>
       </c>
       <c r="L194">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M194">
         <v>330</v>
@@ -14379,7 +14379,7 @@
         <v>2</v>
       </c>
       <c r="L195">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="M195">
         <v>309</v>
@@ -14447,7 +14447,7 @@
         <v>2</v>
       </c>
       <c r="L196">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M196">
         <v>322</v>
@@ -14515,7 +14515,7 @@
         <v>2</v>
       </c>
       <c r="L197">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="M197">
         <v>350</v>
@@ -14583,7 +14583,7 @@
         <v>2</v>
       </c>
       <c r="L198">
-        <v>2</v>
+        <v>4.1</v>
       </c>
       <c r="M198">
         <v>324</v>
@@ -14651,7 +14651,7 @@
         <v>2</v>
       </c>
       <c r="L199">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M199">
         <v>350</v>
@@ -14719,7 +14719,7 @@
         <v>4</v>
       </c>
       <c r="L200">
-        <v>4</v>
+        <v>5.8</v>
       </c>
       <c r="M200">
         <v>226</v>
@@ -14787,7 +14787,7 @@
         <v>2</v>
       </c>
       <c r="L201">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M201">
         <v>350</v>
@@ -14855,7 +14855,7 @@
         <v>2</v>
       </c>
       <c r="L202">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="M202">
         <v>325</v>
@@ -14923,7 +14923,7 @@
         <v>2</v>
       </c>
       <c r="L203">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="M203">
         <v>338</v>
@@ -14991,7 +14991,7 @@
         <v>2</v>
       </c>
       <c r="L204">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M204">
         <v>350</v>
@@ -15059,7 +15059,7 @@
         <v>2</v>
       </c>
       <c r="L205">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M205">
         <v>320</v>
@@ -15127,7 +15127,7 @@
         <v>2</v>
       </c>
       <c r="L206">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="M206">
         <v>340</v>
@@ -15195,7 +15195,7 @@
         <v>3</v>
       </c>
       <c r="L207">
-        <v>3</v>
+        <v>7.3</v>
       </c>
       <c r="M207">
         <v>215</v>
@@ -15263,7 +15263,7 @@
         <v>2</v>
       </c>
       <c r="L208">
-        <v>2</v>
+        <v>6.2</v>
       </c>
       <c r="M208">
         <v>240</v>
@@ -15331,7 +15331,7 @@
         <v>2</v>
       </c>
       <c r="L209">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M209">
         <v>330</v>
@@ -15399,7 +15399,7 @@
         <v>2</v>
       </c>
       <c r="L210">
-        <v>2</v>
+        <v>3.7</v>
       </c>
       <c r="M210">
         <v>325</v>
@@ -15467,7 +15467,7 @@
         <v>2</v>
       </c>
       <c r="L211">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="M211">
         <v>350</v>
@@ -15535,7 +15535,7 @@
         <v>2</v>
       </c>
       <c r="L212">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="M212">
         <v>320</v>
@@ -15603,7 +15603,7 @@
         <v>2</v>
       </c>
       <c r="L213">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M213">
         <v>307</v>
@@ -15671,7 +15671,7 @@
         <v>2</v>
       </c>
       <c r="L214">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="M214">
         <v>338</v>
@@ -15739,7 +15739,7 @@
         <v>2</v>
       </c>
       <c r="L215">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M215">
         <v>298</v>
@@ -15807,7 +15807,7 @@
         <v>2</v>
       </c>
       <c r="L216">
-        <v>2</v>
+        <v>3.7</v>
       </c>
       <c r="M216">
         <v>325</v>
@@ -15875,7 +15875,7 @@
         <v>4</v>
       </c>
       <c r="L217">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M217">
         <v>155</v>
@@ -15943,7 +15943,7 @@
         <v>2</v>
       </c>
       <c r="L218">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="M218">
         <v>330</v>
@@ -16011,7 +16011,7 @@
         <v>2</v>
       </c>
       <c r="L219">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M219">
         <v>306</v>
@@ -16079,7 +16079,7 @@
         <v>2</v>
       </c>
       <c r="L220">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="M220">
         <v>324</v>
@@ -16147,7 +16147,7 @@
         <v>2</v>
       </c>
       <c r="L221">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M221">
         <v>320</v>
@@ -16215,7 +16215,7 @@
         <v>2</v>
       </c>
       <c r="L222">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M222">
         <v>385</v>
@@ -16283,7 +16283,7 @@
         <v>2</v>
       </c>
       <c r="L223">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="M223">
         <v>325</v>
@@ -16351,7 +16351,7 @@
         <v>2</v>
       </c>
       <c r="L224">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M224">
         <v>340</v>
@@ -16419,7 +16419,7 @@
         <v>2</v>
       </c>
       <c r="L225">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="M225">
         <v>345</v>
@@ -16487,7 +16487,7 @@
         <v>2</v>
       </c>
       <c r="L226">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M226">
         <v>325</v>
@@ -16555,7 +16555,7 @@
         <v>2</v>
       </c>
       <c r="L227">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M227">
         <v>355</v>
@@ -16623,7 +16623,7 @@
         <v>2</v>
       </c>
       <c r="L228">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M228">
         <v>330</v>
@@ -16691,7 +16691,7 @@
         <v>2</v>
       </c>
       <c r="L229">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="M229">
         <v>335</v>
@@ -16759,7 +16759,7 @@
         <v>2</v>
       </c>
       <c r="L230">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M230">
         <v>342</v>
@@ -16827,7 +16827,7 @@
         <v>2</v>
       </c>
       <c r="L231">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="M231">
         <v>310</v>
@@ -16895,7 +16895,7 @@
         <v>2</v>
       </c>
       <c r="L232">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M232">
         <v>325</v>
@@ -16963,7 +16963,7 @@
         <v>2</v>
       </c>
       <c r="L233">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="M233">
         <v>380</v>
@@ -17031,7 +17031,7 @@
         <v>2</v>
       </c>
       <c r="L234">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="M234">
         <v>420</v>
@@ -17099,7 +17099,7 @@
         <v>2</v>
       </c>
       <c r="L235">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M235">
         <v>370</v>
@@ -17167,7 +17167,7 @@
         <v>2</v>
       </c>
       <c r="L236">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="M236">
         <v>492</v>
@@ -17235,7 +17235,7 @@
         <v>3</v>
       </c>
       <c r="L237">
-        <v>3</v>
+        <v>3.9</v>
       </c>
       <c r="M237">
         <v>332</v>
@@ -17303,7 +17303,7 @@
         <v>4</v>
       </c>
       <c r="L238">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="M238">
         <v>250</v>
@@ -17371,7 +17371,7 @@
         <v>4</v>
       </c>
       <c r="L239">
-        <v>4</v>
+        <v>2.8</v>
       </c>
       <c r="M239">
         <v>260</v>
@@ -17439,7 +17439,7 @@
         <v>2</v>
       </c>
       <c r="L240">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M240">
         <v>249</v>
@@ -17507,7 +17507,7 @@
         <v>2</v>
       </c>
       <c r="L241">
-        <v>2</v>
+        <v>4.1</v>
       </c>
       <c r="M241">
         <v>259</v>
@@ -17575,7 +17575,7 @@
         <v>2</v>
       </c>
       <c r="L242">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M242">
         <v>300</v>
@@ -17643,7 +17643,7 @@
         <v>2</v>
       </c>
       <c r="L243">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M243">
         <v>305</v>
@@ -17711,7 +17711,7 @@
         <v>2</v>
       </c>
       <c r="L244">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M244">
         <v>290</v>
@@ -17779,7 +17779,7 @@
         <v>2</v>
       </c>
       <c r="L245">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M245">
         <v>300</v>
@@ -17847,7 +17847,7 @@
         <v>2</v>
       </c>
       <c r="L246">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M246">
         <v>295</v>
@@ -17915,7 +17915,7 @@
         <v>2</v>
       </c>
       <c r="L247">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M247">
         <v>330</v>
@@ -17983,7 +17983,7 @@
         <v>2</v>
       </c>
       <c r="L248">
-        <v>2</v>
+        <v>4.9</v>
       </c>
       <c r="M248">
         <v>305</v>
@@ -18051,7 +18051,7 @@
         <v>2</v>
       </c>
       <c r="L249">
-        <v>2</v>
+        <v>3.7</v>
       </c>
       <c r="M249">
         <v>304</v>
@@ -18119,7 +18119,7 @@
         <v>2</v>
       </c>
       <c r="L250">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="M250">
         <v>280</v>
@@ -18187,7 +18187,7 @@
         <v>2</v>
       </c>
       <c r="L251">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M251">
         <v>360</v>
@@ -18255,7 +18255,7 @@
         <v>2</v>
       </c>
       <c r="L252">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M252">
         <v>330</v>
@@ -18323,7 +18323,7 @@
         <v>2</v>
       </c>
       <c r="L253">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M253">
         <v>283</v>
@@ -18391,7 +18391,7 @@
         <v>2</v>
       </c>
       <c r="L254">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M254">
         <v>310</v>
@@ -18459,7 +18459,7 @@
         <v>2</v>
       </c>
       <c r="L255">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="M255">
         <v>320</v>

</xml_diff>